<commit_message>
update for OP accesscnt-daily-bysecond
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/exporter/accesscnt-daily-bysecond.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/exporter/accesscnt-daily-bysecond.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -240,6 +240,10 @@
   </si>
   <si>
     <t>select tt.ts as `时间`, tt.ts_cnt as `秒并发`, tt.url, count(tt.url) as `URL并发` from (select t.ts, t.url, gb_ts.ts_cnt from ${moduleName} t inner join (select ts, count(ts) as ts_cnt from ${moduleName} where ts &gt;= str_to_date('${selectedDate} 00:00:00','%Y-%m-%d %H:%i:%s') and ts &lt;= str_to_date('${selectedDate} 23:59:59','%Y-%m-%d %H:%i:%s')  group by ts order by ts_cnt desc limit ${topN}) gb_ts on t.ts = gb_ts.ts) tt group by tt.url, tt.ts, tt.ts_cnt having `URL并发` &gt; ${threshold} order by tt.ts_cnt desc, `URL并发` desc;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -904,10 +908,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.2706123974558448E-2"/>
+          <c:x val="5.2706123974558462E-2"/>
           <c:y val="4.0864285903655984E-2"/>
-          <c:w val="0.83750698680032098"/>
-          <c:h val="0.80433945756780489"/>
+          <c:w val="0.83750698680032087"/>
+          <c:h val="0.80433945756780501"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -952,11 +956,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80622720"/>
-        <c:axId val="80624256"/>
+        <c:axId val="81474304"/>
+        <c:axId val="81475840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80622720"/>
+        <c:axId val="81474304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,14 +969,14 @@
         <c:numFmt formatCode="h:mm:ss;@" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80624256"/>
+        <c:crossAx val="81475840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80624256"/>
+        <c:axId val="81475840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +985,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80622720"/>
+        <c:crossAx val="81474304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -999,7 +1003,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001354" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001354" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1379,10 +1383,13 @@
     <col min="9" max="9" width="2.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="3.75" customHeight="1">
+    <row r="1" spans="2:6" ht="3.75" customHeight="1">
       <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="2:5">
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
       <c r="B2" s="35" t="str">
         <f>"Top"&amp;_settings!$C11&amp;"每秒并发数趋势图"</f>
         <v>Top50每秒并发数趋势图</v>
@@ -1390,49 +1397,49 @@
       <c r="C2" s="35"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:6">
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:6">
       <c r="B4" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="2:5" ht="3" customHeight="1">
+    <row r="5" spans="2:6" ht="3" customHeight="1">
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:6">
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:6">
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:6">
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:6">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10" spans="2:6">
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:6">
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:6">
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:6">
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:6">
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:6">
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:6">
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="2:5">

</xml_diff>